<commit_message>
Form Advance, Form Mask, Form Validation Added
</commit_message>
<xml_diff>
--- a/admin/plan/BCM Planing.xlsx
+++ b/admin/plan/BCM Planing.xlsx
@@ -506,6 +506,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -513,7 +517,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -534,9 +537,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -824,7 +824,7 @@
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -846,241 +846,248 @@
       <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="O1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="10"/>
       <c r="F9" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
     </row>
     <row r="22" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="12"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="13"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="15"/>
+      <c r="A23" s="14"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="16"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+      <c r="A27" s="5"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A24:E24"/>
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="A25:E25"/>
+    <mergeCell ref="A26:E26"/>
     <mergeCell ref="A20:E20"/>
     <mergeCell ref="A21:E21"/>
     <mergeCell ref="A29:E29"/>
@@ -1097,13 +1104,6 @@
     <mergeCell ref="A16:E16"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A24:E24"/>
-    <mergeCell ref="A27:E27"/>
-    <mergeCell ref="A25:E25"/>
-    <mergeCell ref="A26:E26"/>
-    <mergeCell ref="A28:E28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Blood Donation file added and modify Donorinfo
</commit_message>
<xml_diff>
--- a/admin/plan/BCM Planing.xlsx
+++ b/admin/plan/BCM Planing.xlsx
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="75">
   <si>
     <t>Front End</t>
   </si>
@@ -630,16 +630,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -662,10 +658,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -951,7 +951,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,19 +977,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1203,9 +1203,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>24</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="C9" t="s">
         <v>46</v>
@@ -1298,58 +1301,58 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="16" t="s">
+      <c r="A20" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="10"/>
-      <c r="C23" s="11"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="9"/>
     </row>
     <row r="24" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="13"/>
-      <c r="C24" s="14"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="A28" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
@@ -1394,18 +1397,18 @@
       <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
@@ -1415,16 +1418,16 @@
       <c r="C37" s="4"/>
     </row>
     <row r="38" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
@@ -1434,14 +1437,14 @@
       <c r="C40" s="4"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="3"/>
-      <c r="B41" s="3"/>
-      <c r="C41" s="3"/>
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
@@ -1454,12 +1457,21 @@
       <c r="C44" s="4"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A22:C22"/>
     <mergeCell ref="A43:C43"/>
     <mergeCell ref="A44:C44"/>
     <mergeCell ref="A45:C45"/>
@@ -1476,15 +1488,6 @@
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1511,15 +1514,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
User file added and also modified Donorinfo
</commit_message>
<xml_diff>
--- a/admin/plan/BCM Planing.xlsx
+++ b/admin/plan/BCM Planing.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="75">
   <si>
     <t>Front End</t>
   </si>
@@ -448,7 +448,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -633,9 +633,16 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -656,13 +663,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -951,7 +951,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,19 +977,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1226,12 +1226,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
       <c r="C10" t="s">
         <v>47</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="E10" t="s">
         <v>24</v>
@@ -1306,172 +1309,163 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
     </row>
     <row r="24" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="12"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
     </row>
     <row r="38" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A22:C22"/>
     <mergeCell ref="A43:C43"/>
     <mergeCell ref="A44:C44"/>
     <mergeCell ref="A45:C45"/>
@@ -1488,6 +1482,15 @@
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Blood club inof file added
</commit_message>
<xml_diff>
--- a/admin/plan/BCM Planing.xlsx
+++ b/admin/plan/BCM Planing.xlsx
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="75">
   <si>
     <t>Front End</t>
   </si>
@@ -633,16 +633,9 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -663,6 +656,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -951,7 +951,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,19 +977,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1278,9 +1278,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>72</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -1309,163 +1312,172 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
+      <c r="A22" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="11"/>
-      <c r="C23" s="12"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="9"/>
     </row>
     <row r="24" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="14"/>
-      <c r="C24" s="15"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="12"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
+      <c r="A27" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="13"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
     </row>
     <row r="38" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
+      <c r="A38" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="4"/>
-      <c r="C38" s="4"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="4"/>
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="5"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
+      <c r="A43" s="4"/>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
+      <c r="A44" s="4"/>
+      <c r="B44" s="4"/>
+      <c r="C44" s="4"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A22:C22"/>
     <mergeCell ref="A43:C43"/>
     <mergeCell ref="A44:C44"/>
     <mergeCell ref="A45:C45"/>
@@ -1482,15 +1494,6 @@
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Campaign Request and Feedback file added
</commit_message>
<xml_diff>
--- a/admin/plan/BCM Planing.xlsx
+++ b/admin/plan/BCM Planing.xlsx
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="75">
   <si>
     <t>Front End</t>
   </si>
@@ -633,9 +633,16 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -656,13 +663,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -951,7 +951,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,19 +977,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1180,7 +1180,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>23</v>
       </c>
@@ -1195,6 +1195,9 @@
       </c>
       <c r="E8" t="s">
         <v>57</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="G8" t="s">
         <v>51</v>
@@ -1243,7 +1246,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -1253,10 +1256,16 @@
       <c r="E11" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H11" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="E12" t="s">
         <v>26</v>
@@ -1312,172 +1321,163 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="14"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="8"/>
-      <c r="C23" s="9"/>
+      <c r="B23" s="11"/>
+      <c r="C23" s="12"/>
     </row>
     <row r="24" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="12"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="15"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
+      <c r="A32" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="14"/>
+      <c r="B35" s="8"/>
+      <c r="C35" s="8"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="6" t="s">
+      <c r="A36" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
     </row>
     <row r="38" spans="1:3" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="A40" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
+      <c r="A42" s="4"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
+      <c r="A43" s="5"/>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="4"/>
-      <c r="B44" s="4"/>
-      <c r="C44" s="4"/>
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="5"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A22:C22"/>
     <mergeCell ref="A43:C43"/>
     <mergeCell ref="A44:C44"/>
     <mergeCell ref="A45:C45"/>
@@ -1494,6 +1494,15 @@
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Form Transfer in Modal and Table Added For Showing Donor List with action button
</commit_message>
<xml_diff>
--- a/admin/plan/BCM Planing.xlsx
+++ b/admin/plan/BCM Planing.xlsx
@@ -218,7 +218,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="73">
   <si>
     <t>Front End</t>
   </si>
@@ -277,18 +277,9 @@
     <t>Donation</t>
   </si>
   <si>
-    <t>Request Blood</t>
-  </si>
-  <si>
-    <t>Blood Club Info</t>
-  </si>
-  <si>
     <t>Feedback</t>
   </si>
   <si>
-    <t>Campaign Request</t>
-  </si>
-  <si>
     <t>Division</t>
   </si>
   <si>
@@ -403,9 +394,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>BloodDonation</t>
-  </si>
-  <si>
     <t>DonationDate</t>
   </si>
   <si>
@@ -440,6 +428,15 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>BloodDonInfo</t>
+  </si>
+  <si>
+    <t>BloodRequest</t>
+  </si>
+  <si>
+    <t>CampRequest</t>
   </si>
 </sst>
 </file>
@@ -515,7 +512,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -590,17 +587,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14999847407452621"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -610,24 +596,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -639,15 +621,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -931,7 +915,7 @@
   <dimension ref="A1:K45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -945,8 +929,8 @@
     <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" customWidth="1"/>
     <col min="12" max="12" width="16.5546875" customWidth="1"/>
     <col min="13" max="13" width="12.88671875" customWidth="1"/>
     <col min="14" max="14" width="13.44140625" customWidth="1"/>
@@ -957,434 +941,545 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>22</v>
+        <v>72</v>
       </c>
       <c r="I2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H9" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G3" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4" t="s">
-        <v>42</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" t="s">
-        <v>41</v>
-      </c>
-      <c r="I4" t="s">
-        <v>65</v>
-      </c>
-      <c r="J4" t="s">
-        <v>67</v>
-      </c>
-      <c r="K4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" t="s">
-        <v>59</v>
-      </c>
-      <c r="H5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" t="s">
-        <v>66</v>
-      </c>
-      <c r="K5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G6" t="s">
-        <v>60</v>
-      </c>
-      <c r="H6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G8" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="E11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="B18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="15"/>
+      <c r="F18" s="15"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="15"/>
+      <c r="I18" s="15"/>
+      <c r="J18" s="15"/>
+      <c r="K18" s="15"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="13" t="s">
+      <c r="B22" s="13"/>
+      <c r="C22" s="13"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B23" s="14"/>
-      <c r="C23" s="15"/>
-    </row>
-    <row r="24" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="10" t="s">
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="11"/>
-      <c r="C24" s="12"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="B24" s="9"/>
+      <c r="C24" s="10"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="8" t="s">
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="8" t="s">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="8" t="s">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="8" t="s">
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="8" t="s">
+      <c r="A33" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="13"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="9" t="s">
+      <c r="A36" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
     </row>
     <row r="38" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
@@ -1399,11 +1494,11 @@
       <c r="C39" s="3"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="3"/>
@@ -1416,14 +1511,14 @@
       <c r="C42" s="3"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" s="3"/>
@@ -1432,6 +1527,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A22:C22"/>
     <mergeCell ref="A43:C43"/>
     <mergeCell ref="A44:C44"/>
     <mergeCell ref="A45:C45"/>
@@ -1443,20 +1547,11 @@
     <mergeCell ref="A30:C30"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A22:C22"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="A35:C35"/>
     <mergeCell ref="A37:C37"/>
     <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A42:C42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
@@ -1483,43 +1578,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="A1" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" t="s">
         <v>28</v>
       </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" t="s">
-        <v>31</v>
-      </c>
       <c r="I2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>